<commit_message>
Started work on the MC simulations for uncertainty around reading times
</commit_message>
<xml_diff>
--- a/Types.xlsx
+++ b/Types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_proj\email_dash1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA44FE3-F69C-48AF-8ADB-3267996DEFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1283DCC2-B364-46D1-A39F-3C890E7BE85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Size of Team</t>
   </si>
@@ -44,16 +44,7 @@
     <t>Period size (days)</t>
   </si>
   <si>
-    <t>Type 1</t>
-  </si>
-  <si>
     <t>Type 2</t>
-  </si>
-  <si>
-    <t>Reading time (seconds)</t>
-  </si>
-  <si>
-    <t>Number of emails sent per person per period</t>
   </si>
   <si>
     <t>Average number of recipients for each email</t>
@@ -68,24 +59,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Person: Total time reading emails (mins)</t>
-  </si>
-  <si>
-    <t>Essential (mins)</t>
-  </si>
-  <si>
-    <t>Non Essential (mins)</t>
-  </si>
-  <si>
-    <t>Staff: Total time reading emails (hours)</t>
-  </si>
-  <si>
-    <t>Essential (hours)</t>
-  </si>
-  <si>
-    <t>Non Essential (hours)</t>
-  </si>
-  <si>
     <t>Average pay per hour</t>
   </si>
   <si>
@@ -93,6 +66,39 @@
   </si>
   <si>
     <t>Type 3 - everyone</t>
+  </si>
+  <si>
+    <t>Staff: Total time (hours)</t>
+  </si>
+  <si>
+    <t>Time per email</t>
+  </si>
+  <si>
+    <t>Read (seconds)</t>
+  </si>
+  <si>
+    <t>Type 1 - single person</t>
+  </si>
+  <si>
+    <t>Action (mins)</t>
+  </si>
+  <si>
+    <t>Respond/write (mins)</t>
+  </si>
+  <si>
+    <t>Total time (mins)</t>
+  </si>
+  <si>
+    <t>Person: Total time (hours)</t>
+  </si>
+  <si>
+    <t>Essential</t>
+  </si>
+  <si>
+    <t>Non Essential</t>
+  </si>
+  <si>
+    <t>Number of emails sent per person</t>
   </si>
 </sst>
 </file>
@@ -164,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -423,90 +429,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -569,79 +491,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -651,23 +553,56 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="6" fontId="1" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="1" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="1" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -686,8 +621,92 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +745,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -739,8 +758,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-AU" sz="3000" baseline="0"/>
-              <a:t>Total Time reading emails</a:t>
+              <a:rPr lang="en-AU" sz="2400" baseline="0"/>
+              <a:t>Total Time in emails</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -758,7 +777,308 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B790-4F2D-9B49-0360CEA84072}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B790-4F2D-9B49-0360CEA84072}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$18:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Essential</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non Essential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$18:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D398-4729-B4C7-0038F2025D95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU" sz="2400" baseline="0"/>
+              <a:t>Total Time in emails</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -812,47 +1132,125 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$14:$B$15</c:f>
+              <c:f>Sheet1!$C$6:$E$6</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Essential (mins)</c:v>
+                  <c:v>Type 1 - single person</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Non Essential (mins)</c:v>
+                  <c:v>Type 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Type 3 - everyone</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$F$15</c:f>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>34.67</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.000000000000002</c:v>
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D398-4729-B4C7-0038F2025D95}"/>
+              <c16:uniqueId val="{00000000-EF81-4159-AF43-7DFC885AA92B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -880,8 +1278,8 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -981,7 +1379,566 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1505,15 +2462,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>179916</xdr:colOff>
+      <xdr:colOff>411238</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>179918</xdr:rowOff>
+      <xdr:rowOff>193525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>200026</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1533,6 +2490,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>385080</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>244929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68658BC-7348-8D78-F415-73C572B4033A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1804,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="V18" sqref="U18:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75" x14ac:dyDescent="0.5"/>
@@ -1816,311 +2809,376 @@
     <col min="2" max="2" width="96.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4">
-        <v>14</v>
+      <c r="B2" s="32"/>
+      <c r="C2" s="24">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="54">
+      <c r="B3" s="34"/>
+      <c r="C3" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="55">
-        <v>30</v>
+      <c r="A4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="26">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="6" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="6" t="s">
+    <row r="6" spans="1:6" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="67"/>
+      <c r="C6" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
+      <c r="E6" s="65" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A7" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="8">
+      <c r="A7" s="51"/>
+      <c r="B7" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="56">
         <v>60</v>
       </c>
-      <c r="D7" s="9">
-        <v>10</v>
-      </c>
-      <c r="E7" s="27">
-        <v>30</v>
-      </c>
-      <c r="F7" s="15"/>
+      <c r="D7" s="57">
+        <v>20</v>
+      </c>
+      <c r="E7" s="58">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="59">
         <v>5</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="10">
-        <v>20</v>
-      </c>
-      <c r="D8" s="11">
-        <v>10</v>
-      </c>
-      <c r="E8" s="28">
+      <c r="D8" s="60">
         <v>2</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="E8" s="61">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A9" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="10">
+    <row r="9" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="51"/>
+      <c r="B9" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="68">
+        <v>2</v>
+      </c>
+      <c r="D9" s="50">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
-        <v>10</v>
-      </c>
-      <c r="E9" s="12">
-        <f>C2-1</f>
-        <v>13</v>
-      </c>
-      <c r="F9" s="15"/>
+      <c r="E9" s="53">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="E10" s="29">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15"/>
+      <c r="A10" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="62">
+        <f>ROUND((C7/60)+C8+C9,2)</f>
+        <v>8</v>
+      </c>
+      <c r="D10" s="54">
+        <f>ROUND((D7/60)+D8+D9,2)</f>
+        <v>3.33</v>
+      </c>
+      <c r="E10" s="55">
+        <f>ROUND((E7/60)+E8+E9,2)</f>
+        <v>1.25</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="34" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11" s="48"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="24">
-        <f>C8*C9</f>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A12" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="16">
-        <f>D8*D9</f>
-        <v>100</v>
-      </c>
-      <c r="E12" s="38">
-        <f>E8*E9</f>
-        <v>26</v>
-      </c>
-      <c r="F12" s="36">
-        <f>SUM(C12:E12)</f>
-        <v>146</v>
-      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="43">
+        <v>15</v>
+      </c>
+      <c r="D12" s="44">
+        <v>10</v>
+      </c>
+      <c r="E12" s="45">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="24">
-        <f>ROUND((C12*C7)/60, 2)</f>
-        <v>20</v>
-      </c>
-      <c r="D13" s="16">
-        <f t="shared" ref="D13:E13" si="0">ROUND((D12*D7)/60, 2)</f>
-        <v>16.670000000000002</v>
-      </c>
-      <c r="E13" s="38">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F13" s="17">
-        <f>SUM(C13:E13)</f>
-        <v>49.67</v>
-      </c>
+      <c r="A13" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="72">
+        <v>1</v>
+      </c>
+      <c r="D13" s="27">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <f>C2-1</f>
+        <v>14</v>
+      </c>
+      <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A14" s="18"/>
-      <c r="B14" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="25">
-        <f>ROUND((C12*C10*C7)/60,2)</f>
-        <v>20</v>
-      </c>
-      <c r="D14" s="19">
-        <f t="shared" ref="D14:E14" si="1">ROUND((D12*D10*D7)/60,2)</f>
-        <v>1.67</v>
-      </c>
-      <c r="E14" s="39">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="F14" s="20">
-        <f t="shared" ref="F14:F15" si="2">SUM(C14:E14)</f>
-        <v>34.67</v>
-      </c>
+    <row r="14" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="28">
+        <v>1</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0.7</v>
+      </c>
+      <c r="E14" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="21"/>
-      <c r="B15" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="26">
-        <f>C13-C14</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="22">
-        <f t="shared" ref="D15:E15" si="3">D13-D14</f>
-        <v>15.000000000000002</v>
-      </c>
-      <c r="E15" s="42">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="23">
-        <f t="shared" si="2"/>
-        <v>15.000000000000002</v>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="25">
-        <f>ROUND((C13*$C$2)/60, 2)</f>
-        <v>4.67</v>
-      </c>
-      <c r="D16" s="19">
-        <f>ROUND((D13*$C$2)/60, 2)</f>
-        <v>3.89</v>
-      </c>
-      <c r="E16" s="39">
-        <f>ROUND((E13*$C$2)/60, 2)</f>
-        <v>3.03</v>
-      </c>
-      <c r="F16" s="37">
-        <f>ROUND((F13*$C$2)/60, 2)</f>
-        <v>11.59</v>
+        <v>5</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="11">
+        <f>C12*C13</f>
+        <v>15</v>
+      </c>
+      <c r="D16" s="4">
+        <f>D12*D13</f>
+        <v>30</v>
+      </c>
+      <c r="E16" s="19">
+        <f>E12*E13</f>
+        <v>28</v>
+      </c>
+      <c r="F16" s="18">
+        <f>SUM(C16:E16)</f>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17" s="18"/>
-      <c r="B17" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="25">
-        <f>ROUND((C14*$C$2)/60, 2)</f>
-        <v>4.67</v>
-      </c>
-      <c r="D17" s="19">
-        <f>ROUND((D14*$C$2)/60, 2)</f>
-        <v>0.39</v>
-      </c>
-      <c r="E17" s="39">
-        <f>ROUND((E14*$C$2)/60, 2)</f>
-        <v>3.03</v>
-      </c>
-      <c r="F17" s="37">
-        <f>ROUND((F14*$C$2)/60, 2)</f>
-        <v>8.09</v>
+      <c r="A17" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="11">
+        <f>ROUND((C16*C10+(C12*C9))/60, 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="4">
+        <f>ROUND((D16*D10+(D12*D9))/60, 2)</f>
+        <v>1.83</v>
+      </c>
+      <c r="E17" s="19">
+        <f t="shared" ref="D17:E17" si="0">ROUND((E16*E10+(E12*E9))/60, 2)</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F17" s="5">
+        <f>SUM(C17:E17)</f>
+        <v>4.91</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="18"/>
-      <c r="B18" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="25">
-        <f>ROUND((C15*$C$2)/60, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="19">
-        <f>ROUND((D15*$C$2)/60, 2)</f>
-        <v>3.5</v>
-      </c>
-      <c r="E18" s="39">
-        <f>ROUND((E15*$C$2)/60, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="37">
-        <f>ROUND((F15*$C$2)/60, 2)</f>
-        <v>3.5</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18" s="6"/>
+      <c r="B18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="12">
+        <f>ROUND((C16*C14*C10+(C12*C9))/60,2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D18" s="49">
+        <f t="shared" ref="D18:E18" si="1">ROUND((D16*D14*D10+(D12*D9))/60,2)</f>
+        <v>1.33</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" ref="F18:F19" si="2">SUM(C18:E18)</f>
+        <v>3.89</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44">
-        <f>C18*$C$4*(260/$C$3)</f>
+      <c r="A19" s="8"/>
+      <c r="B19" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="13">
+        <f>C17-C18</f>
         <v>0</v>
       </c>
-      <c r="D19" s="45">
-        <f t="shared" ref="D19:F19" si="4">D18*$C$4*(260/$C$3)</f>
-        <v>27300</v>
-      </c>
-      <c r="E19" s="46">
+      <c r="D19" s="9">
+        <f t="shared" ref="D19:E19" si="3">D17-D18</f>
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" si="3"/>
+        <v>0.52</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="2"/>
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A20" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="12">
+        <f>ROUND(C17*$C$2, 2)</f>
+        <v>37.5</v>
+      </c>
+      <c r="D20" s="49">
+        <f t="shared" ref="D20:E20" si="4">ROUND(D17*$C$2, 2)</f>
+        <v>27.45</v>
+      </c>
+      <c r="E20" s="20">
         <f t="shared" si="4"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F20" s="7">
+        <f>ROUND(F17*$C$2, 2)</f>
+        <v>73.650000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A21" s="6"/>
+      <c r="B21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="12">
+        <f>ROUND(C18*$C$2, 2)</f>
+        <v>37.5</v>
+      </c>
+      <c r="D21" s="49">
+        <f t="shared" ref="D21:F21" si="5">ROUND(D18*$C$2, 2)</f>
+        <v>19.95</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="5"/>
+        <v>0.9</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="5"/>
+        <v>58.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="6"/>
+      <c r="B22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="13">
+        <f>ROUND(C19*$C$2, 2)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="47">
-        <f>F18*$C$4*(260/$C$3)</f>
-        <v>27300</v>
+      <c r="D22" s="9">
+        <f t="shared" ref="D22:F22" si="6">ROUND(D19*$C$2, 2)</f>
+        <v>7.5</v>
+      </c>
+      <c r="E22" s="22">
+        <f t="shared" si="6"/>
+        <v>7.8</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="6"/>
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="69">
+        <f>C22*$C$4*(260/$C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="70">
+        <f>D22*$C$4*(260/$C$3)</f>
+        <v>156000</v>
+      </c>
+      <c r="E23" s="71">
+        <f t="shared" ref="D23:E23" si="7">E22*$C$4*(260/$C$3)</f>
+        <v>162240</v>
+      </c>
+      <c r="F23" s="23">
+        <f>F22*$C$4*(260/$C$3)</f>
+        <v>318240</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAJOR: With simulation behind the scenes
</commit_message>
<xml_diff>
--- a/Types.xlsx
+++ b/Types.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_proj\email_dash1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1283DCC2-B364-46D1-A39F-3C890E7BE85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B890E-B9BA-4258-B38E-8E5B29140691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Size of Team</t>
   </si>
@@ -99,6 +100,30 @@
   </si>
   <si>
     <t>Number of emails sent per person</t>
+  </si>
+  <si>
+    <t>Emails received</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Best Guess</t>
+  </si>
+  <si>
+    <t>Read time</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t>Type 3</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -585,42 +610,6 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -633,23 +622,23 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -675,7 +664,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -689,12 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -706,6 +689,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,6 +1141,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7848-43E6-9ABA-7BB5740277C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1131,6 +1161,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7848-43E6-9ABA-7BB5740277C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1146,6 +1181,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7848-43E6-9ABA-7BB5740277C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2800,7 +2840,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="V18" sqref="U18:V18"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75" x14ac:dyDescent="0.5"/>
@@ -2816,19 +2856,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="24">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="25">
         <v>1</v>
       </c>
@@ -2844,117 +2884,117 @@
     </row>
     <row r="5" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="6" spans="1:6" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="63" t="s">
+      <c r="B6" s="72"/>
+      <c r="C6" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="53" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="44">
         <v>60</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="45">
         <v>20</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="46">
         <v>15</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="47">
         <v>5</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="48">
         <v>2</v>
       </c>
-      <c r="E8" s="61">
+      <c r="E8" s="49">
         <v>1</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="54">
         <v>2</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="38">
         <v>1</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="41">
         <v>0</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="62">
+      <c r="B10" s="60"/>
+      <c r="C10" s="50">
         <f>ROUND((C7/60)+C8+C9,2)</f>
         <v>8</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="42">
         <f>ROUND((D7/60)+D8+D9,2)</f>
         <v>3.33</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="43">
         <f>ROUND((E7/60)+E8+E9,2)</f>
         <v>1.25</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="48"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="43">
+      <c r="B12" s="62"/>
+      <c r="C12" s="31">
         <v>15</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="32">
         <v>10</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="33">
         <v>2</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="72">
+      <c r="B13" s="64"/>
+      <c r="C13" s="58">
         <v>1</v>
       </c>
       <c r="D13" s="27">
@@ -2967,10 +3007,10 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="42"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="28">
         <v>1</v>
       </c>
@@ -2988,10 +3028,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="11">
         <f>C12*C13</f>
         <v>15</v>
@@ -3010,10 +3050,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="11">
         <f>ROUND((C16*C10+(C12*C9))/60, 2)</f>
         <v>2.5</v>
@@ -3023,7 +3063,7 @@
         <v>1.83</v>
       </c>
       <c r="E17" s="19">
-        <f t="shared" ref="D17:E17" si="0">ROUND((E16*E10+(E12*E9))/60, 2)</f>
+        <f t="shared" ref="E17" si="0">ROUND((E16*E10+(E12*E9))/60, 2)</f>
         <v>0.57999999999999996</v>
       </c>
       <c r="F17" s="5">
@@ -3040,7 +3080,7 @@
         <f>ROUND((C16*C14*C10+(C12*C9))/60,2)</f>
         <v>2.5</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="37">
         <f t="shared" ref="D18:E18" si="1">ROUND((D16*D14*D10+(D12*D9))/60,2)</f>
         <v>1.33</v>
       </c>
@@ -3076,15 +3116,15 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="12">
         <f>ROUND(C17*$C$2, 2)</f>
         <v>37.5</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="37">
         <f t="shared" ref="D20:E20" si="4">ROUND(D17*$C$2, 2)</f>
         <v>27.45</v>
       </c>
@@ -3106,7 +3146,7 @@
         <f>ROUND(C18*$C$2, 2)</f>
         <v>37.5</v>
       </c>
-      <c r="D21" s="49">
+      <c r="D21" s="37">
         <f t="shared" ref="D21:F21" si="5">ROUND(D18*$C$2, 2)</f>
         <v>19.95</v>
       </c>
@@ -3142,20 +3182,20 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="69">
+      <c r="B23" s="60"/>
+      <c r="C23" s="55">
         <f>C22*$C$4*(260/$C$3)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="56">
         <f>D22*$C$4*(260/$C$3)</f>
         <v>156000</v>
       </c>
-      <c r="E23" s="71">
-        <f t="shared" ref="D23:E23" si="7">E22*$C$4*(260/$C$3)</f>
+      <c r="E23" s="57">
+        <f t="shared" ref="E23" si="7">E22*$C$4*(260/$C$3)</f>
         <v>162240</v>
       </c>
       <c r="F23" s="23">
@@ -3165,20 +3205,157 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA55607B-654F-471F-AE68-2D8F97D50177}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WORKING: updated pie charts and added functionality
</commit_message>
<xml_diff>
--- a/Types.xlsx
+++ b/Types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_proj\email_dash1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B890E-B9BA-4258-B38E-8E5B29140691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA3201E-37E5-4098-8A49-6DB96DF2504F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -690,6 +690,24 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -713,24 +731,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2840,7 +2840,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75" x14ac:dyDescent="0.5"/>
@@ -2856,19 +2856,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="60"/>
       <c r="C2" s="24">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="25">
         <v>1</v>
       </c>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="5" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="6" spans="1:6" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="51" t="s">
         <v>13</v>
       </c>
@@ -2947,10 +2947,10 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="60"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="50">
         <f>ROUND((C7/60)+C8+C9,2)</f>
         <v>8</v>
@@ -2974,10 +2974,10 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="62"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="31">
         <v>15</v>
       </c>
@@ -2990,10 +2990,10 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="64"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="58">
         <v>1</v>
       </c>
@@ -3007,10 +3007,10 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="66"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="28">
         <v>1</v>
       </c>
@@ -3028,10 +3028,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="68"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="11">
         <f>C12*C13</f>
         <v>15</v>
@@ -3050,10 +3050,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="68"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="11">
         <f>ROUND((C16*C10+(C12*C9))/60, 2)</f>
         <v>2.5</v>
@@ -3116,10 +3116,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="70"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="12">
         <f>ROUND(C17*$C$2, 2)</f>
         <v>37.5</v>
@@ -3182,10 +3182,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="60"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="55">
         <f>C22*$C$4*(260/$C$3)</f>
         <v>0</v>
@@ -3205,17 +3205,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>